<commit_message>
Checked 4th case, had to use wolfram alpha
</commit_message>
<xml_diff>
--- a/4.xlsx
+++ b/4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\TickTock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2AF239-93AA-44AE-A664-AF61AA42A712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6323E4AF-8D6C-443D-9A17-A2C02E8C7203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3723D68D-918B-4440-B198-80EC7C1C3AED}"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="21600" windowHeight="12645" xr2:uid="{3723D68D-918B-4440-B198-80EC7C1C3AED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,10 +112,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -139,22 +140,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>520211</xdr:colOff>
+      <xdr:colOff>271096</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>112102</xdr:rowOff>
+      <xdr:rowOff>124557</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>605936</xdr:colOff>
+      <xdr:colOff>356088</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>26377</xdr:rowOff>
+      <xdr:rowOff>38832</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB337F76-0D53-51FF-790F-39AB61C30B67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3258528C-C97D-5CB3-7330-3586141AA31B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -177,8 +178,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7517423" y="1255102"/>
-          <a:ext cx="3126398" cy="3152775"/>
+          <a:off x="8894884" y="1267557"/>
+          <a:ext cx="3125665" cy="3152775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -497,19 +498,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B239FE16-A4D7-466B-8C30-524C702BBC31}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -583,11 +585,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <f>(C2+1-B2)*(E2+1-D2)</f>
         <v>749736694739</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <f>G2*F2</f>
         <v>749736694739</v>
       </c>
@@ -596,8 +598,8 @@
         <v>50515093</v>
       </c>
       <c r="J2" s="2">
-        <f>12*(I2^2-SUM(G:G))+SUM(H:H)</f>
-        <v>2.3967876580415112E+16</v>
+        <f>12*(2551774620798640-SUM(G:G))+SUM(H:H)</f>
+        <v>2.3967876580415004E+16</v>
       </c>
       <c r="M2">
         <v>3034546</v>
@@ -616,7 +618,7 @@
         <v>17678520619155</v>
       </c>
       <c r="R2" t="b">
-        <f>Q2=G7+G8+G9</f>
+        <f>Q2=G3+G5+G9</f>
         <v>1</v>
       </c>
     </row>
@@ -625,31 +627,31 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f>M4</f>
-        <v>3245540</v>
+        <f>M2</f>
+        <v>3034546</v>
       </c>
       <c r="C3">
-        <f>N4</f>
-        <v>21669054</v>
+        <f>M4-1</f>
+        <v>3245539</v>
       </c>
       <c r="D3">
-        <f>O4</f>
-        <v>8801316</v>
+        <f>O2</f>
+        <v>22608053</v>
       </c>
       <c r="E3">
-        <f>O3-1</f>
-        <v>18236821</v>
+        <f>P2</f>
+        <v>23794117</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <f t="shared" ref="G3:G13" si="1">(C3+1-B3)*(E3+1-D3)</f>
-        <v>173835186323590</v>
-      </c>
-      <c r="H3">
+        <v>250252598610</v>
+      </c>
+      <c r="H3" s="2">
         <f t="shared" ref="H3:H13" si="2">G3*F3</f>
-        <v>173835186323590</v>
+        <v>250252598610</v>
       </c>
       <c r="J3">
         <v>2.3967876580415112E+16</v>
@@ -670,8 +672,8 @@
         <f t="shared" si="0"/>
         <v>319759159922533</v>
       </c>
-      <c r="R3" t="b">
-        <f>Q3=G5+G6+G9+G10+G12+G13</f>
+      <c r="R3" s="3" t="b">
+        <f>Q3=G8+G9+G10+G11+G13+G14+G15</f>
         <v>1</v>
       </c>
     </row>
@@ -688,8 +690,8 @@
         <v>10474245</v>
       </c>
       <c r="D4">
-        <f>O3</f>
-        <v>18236822</v>
+        <f>O4</f>
+        <v>8801316</v>
       </c>
       <c r="E4">
         <f>O2-1</f>
@@ -698,13 +700,13 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <f t="shared" si="1"/>
-        <v>31598343757086</v>
-      </c>
-      <c r="H4">
+        <v>99804842592322</v>
+      </c>
+      <c r="H4" s="2">
         <f t="shared" si="2"/>
-        <v>31598343757086</v>
+        <v>99804842592322</v>
       </c>
       <c r="M4">
         <v>3245540</v>
@@ -723,7 +725,7 @@
         <v>505601975505440</v>
       </c>
       <c r="R4" t="b">
-        <f>Q4=SUM(G3:G5)+SUM(G8:G12)</f>
+        <f>Q4=G4+G5+G6+G7+G8+G9+G10+G12+G13</f>
         <v>1</v>
       </c>
     </row>
@@ -732,31 +734,35 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f>M3</f>
-        <v>10474246</v>
+        <f>M4</f>
+        <v>3245540</v>
       </c>
       <c r="C5">
-        <f>N4</f>
-        <v>21669054</v>
+        <f>M3-1</f>
+        <v>10474245</v>
       </c>
       <c r="D5">
-        <f>O3</f>
-        <v>18236822</v>
+        <f>O2</f>
+        <v>22608053</v>
       </c>
       <c r="E5">
-        <f>O2-1</f>
-        <v>22608052</v>
+        <f>P2</f>
+        <v>23794117</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <f t="shared" si="1"/>
-        <v>48935096139879</v>
-      </c>
-      <c r="H5">
+        <v>8573715181890</v>
+      </c>
+      <c r="H5" s="2">
         <f t="shared" si="2"/>
-        <v>97870192279758</v>
+        <v>17147430363780</v>
+      </c>
+      <c r="J5" s="3">
+        <f>SUM(G2:G15)</f>
+        <v>624767355159212</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -764,31 +770,35 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f>N4+1</f>
-        <v>21669055</v>
+        <f>M4</f>
+        <v>3245540</v>
       </c>
       <c r="C6">
-        <f>N3</f>
-        <v>25904962</v>
+        <f>M3-1</f>
+        <v>10474245</v>
       </c>
       <c r="D6">
-        <f>O3</f>
-        <v>18236822</v>
+        <f>P2+1</f>
+        <v>23794118</v>
       </c>
       <c r="E6">
-        <f>P3</f>
-        <v>38959070</v>
+        <f>P4</f>
+        <v>36244611</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <f t="shared" si="1"/>
-        <v>87777540317092</v>
-      </c>
-      <c r="H6">
+        <v>90000960680764</v>
+      </c>
+      <c r="H6" s="2">
         <f t="shared" si="2"/>
-        <v>87777540317092</v>
+        <v>90000960680764</v>
+      </c>
+      <c r="J6" s="3">
+        <f>SUM(H2:H15)</f>
+        <v>843789392741867</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -796,31 +806,34 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f>M2</f>
-        <v>3034546</v>
+        <f>M3</f>
+        <v>10474246</v>
       </c>
       <c r="C7">
-        <f>M4-1</f>
-        <v>3245539</v>
+        <f>N2</f>
+        <v>17939732</v>
       </c>
       <c r="D7">
-        <f>O2</f>
-        <v>22608053</v>
+        <f>O4</f>
+        <v>8801316</v>
       </c>
       <c r="E7">
-        <f>P2</f>
-        <v>23794117</v>
+        <f>O3-1</f>
+        <v>18236821</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <f t="shared" si="1"/>
-        <v>250252598610</v>
-      </c>
-      <c r="H7">
+        <v>70440647381422</v>
+      </c>
+      <c r="H7" s="2">
         <f t="shared" si="2"/>
-        <v>250252598610</v>
+        <v>70440647381422</v>
+      </c>
+      <c r="J7">
+        <v>843789392741867</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -828,31 +841,31 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f>M4</f>
-        <v>3245540</v>
+        <f>M3</f>
+        <v>10474246</v>
       </c>
       <c r="C8">
-        <f>M3-1</f>
-        <v>10474245</v>
+        <f>N2</f>
+        <v>17939732</v>
       </c>
       <c r="D8">
-        <f>O2</f>
-        <v>22608053</v>
+        <f>O3</f>
+        <v>18236822</v>
       </c>
       <c r="E8">
-        <f>P2</f>
-        <v>23794117</v>
+        <f>O2-1</f>
+        <v>22608052</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <f t="shared" si="1"/>
-        <v>8573715181890</v>
-      </c>
-      <c r="H8">
+        <v>32633368204497</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>17147430363780</v>
+        <v>65266736408994</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -878,11 +891,11 @@
       <c r="F9">
         <v>3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <f t="shared" si="1"/>
         <v>8854552838655</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <f t="shared" si="2"/>
         <v>26563658515965</v>
       </c>
@@ -892,31 +905,31 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f>N2+1</f>
-        <v>17939733</v>
+        <f>M3</f>
+        <v>10474246</v>
       </c>
       <c r="C10">
-        <f>N4</f>
-        <v>21669054</v>
+        <f>N2</f>
+        <v>17939732</v>
       </c>
       <c r="D10">
-        <f>O2</f>
-        <v>22608053</v>
+        <f>P2+1</f>
+        <v>23794118</v>
       </c>
       <c r="E10">
-        <f>P2</f>
-        <v>23794117</v>
+        <f>P4</f>
+        <v>36244611</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <f t="shared" si="1"/>
-        <v>4423218297930</v>
-      </c>
-      <c r="H10">
+        <v>92949001100578</v>
+      </c>
+      <c r="H10" s="2">
         <f t="shared" si="2"/>
-        <v>8846436595860</v>
+        <v>185898002201156</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -924,31 +937,31 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <f>M4</f>
-        <v>3245540</v>
+        <f>M3</f>
+        <v>10474246</v>
       </c>
       <c r="C11">
-        <f>M3-1</f>
-        <v>10474245</v>
+        <f>N2</f>
+        <v>17939732</v>
       </c>
       <c r="D11">
-        <f>P2+1</f>
-        <v>23794118</v>
+        <f>P4+1</f>
+        <v>36244612</v>
       </c>
       <c r="E11">
-        <f>P4</f>
-        <v>36244611</v>
+        <f>P3</f>
+        <v>38959070</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>90000960680764</v>
-      </c>
-      <c r="H11">
+        <v>20264758376533</v>
+      </c>
+      <c r="H11" s="2">
         <f t="shared" si="2"/>
-        <v>90000960680764</v>
+        <v>20264758376533</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -956,31 +969,31 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f>M3</f>
-        <v>10474246</v>
+        <f>N2+1</f>
+        <v>17939733</v>
       </c>
       <c r="C12">
         <f>N4</f>
         <v>21669054</v>
       </c>
       <c r="D12">
-        <f>P2+1</f>
-        <v>23794118</v>
+        <f>O4</f>
+        <v>8801316</v>
       </c>
       <c r="E12">
-        <f>P4</f>
-        <v>36244611</v>
+        <f>O3-1</f>
+        <v>18236821</v>
       </c>
       <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="1"/>
-        <v>139380902285646</v>
-      </c>
-      <c r="H12">
+        <v>35188040106932</v>
+      </c>
+      <c r="H12" s="2">
         <f t="shared" si="2"/>
-        <v>278761804571292</v>
+        <v>35188040106932</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -988,31 +1001,95 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f>M3</f>
-        <v>10474246</v>
+        <f>N2+1</f>
+        <v>17939733</v>
       </c>
       <c r="C13">
         <f>N4</f>
         <v>21669054</v>
       </c>
       <c r="D13">
+        <f>O3</f>
+        <v>18236822</v>
+      </c>
+      <c r="E13">
+        <f>P4</f>
+        <v>36244611</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>67156847418380</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="2"/>
+        <v>134313694836760</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f>N2+1</f>
+        <v>17939733</v>
+      </c>
+      <c r="C14">
+        <f>N4</f>
+        <v>21669054</v>
+      </c>
+      <c r="D14">
         <f>P4+1</f>
         <v>36244612</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f>P3</f>
         <v>38959070</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>30387850043331</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>30387850043331</v>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" ref="G14:G15" si="3">(C14+1-B14)*(E14+1-D14)</f>
+        <v>10123091666798</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" ref="H14:H15" si="4">G14*F14</f>
+        <v>10123091666798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>N4+1</f>
+        <v>21669055</v>
+      </c>
+      <c r="C15">
+        <f>N3</f>
+        <v>25904962</v>
+      </c>
+      <c r="D15">
+        <f>O3</f>
+        <v>18236822</v>
+      </c>
+      <c r="E15">
+        <f>P3</f>
+        <v>38959070</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="3"/>
+        <v>87777540317092</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="4"/>
+        <v>87777540317092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>